<commit_message>
New pressure sensor stuff
</commit_message>
<xml_diff>
--- a/Lab Equipment and Etc/Lab Equipment List.xlsx
+++ b/Lab Equipment and Etc/Lab Equipment List.xlsx
@@ -12,7 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17964" windowHeight="8208"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LAB 1" sheetId="1" r:id="rId1"/>
+    <sheet name="LAB 2" sheetId="2" r:id="rId2"/>
+    <sheet name="LAB 3" sheetId="3" r:id="rId3"/>
+    <sheet name="LAB 4" sheetId="4" r:id="rId4"/>
+    <sheet name="LAB 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>MAE 224 Lab Parts List</t>
   </si>
@@ -62,9 +66,6 @@
     <t>Low-Range pressure transducer</t>
   </si>
   <si>
-    <t>HSCDLNN001PDAA3</t>
-  </si>
-  <si>
     <t>Particle Photon</t>
   </si>
   <si>
@@ -81,13 +82,109 @@
   </si>
   <si>
     <t>Keeps pressure spikes from hand pump from reaching pressure transducer</t>
+  </si>
+  <si>
+    <t>HSCDLNN001PDAA3 (+/1 1PSID)</t>
+  </si>
+  <si>
+    <t>Lab 5: Final Project Wind Turbine</t>
+  </si>
+  <si>
+    <t>Lab 4: Airfoil and Cylinder</t>
+  </si>
+  <si>
+    <t>LAB 3: Boundary Layer</t>
+  </si>
+  <si>
+    <t>LAB 2: Pipe Flow</t>
+  </si>
+  <si>
+    <t>Pipe Flow Apparatus with Turbulent and Laminar pipe flows</t>
+  </si>
+  <si>
+    <t>Custom build by Lab technician</t>
+  </si>
+  <si>
+    <t>Total Flow Meter</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/products/833</t>
+  </si>
+  <si>
+    <t>Laminar Flow Meter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Electronic-Water-Counter-Sensor-mim-4-5/dp/B00K7ZWOKC/ref=pd_bxgy_60_img_2?_encoding=UTF8&amp;psc=1&amp;refRID=166NS77ME1MAZEVNPFKM</t>
+  </si>
+  <si>
+    <t>^ Note that this flow meter was calibrated by the Tas in situ, see uploaded calibration sheet</t>
+  </si>
+  <si>
+    <t>Pump driving circuit with flow meter connections</t>
+  </si>
+  <si>
+    <t>See uploaded schematics and drawings for details</t>
+  </si>
+  <si>
+    <t>OPTIONAL: Pressure sensor for reading pressure drop along pipes</t>
+  </si>
+  <si>
+    <t>Facility capable of producing a boundary layer at various velocities</t>
+  </si>
+  <si>
+    <t>Linear servo motor</t>
+  </si>
+  <si>
+    <t>Pitot tube with attachement points for linear servo</t>
+  </si>
+  <si>
+    <t>Low-range pressure sensor</t>
+  </si>
+  <si>
+    <t>We use a small undergraduate wind tunnel with a range of 1-10 m/s or so</t>
+  </si>
+  <si>
+    <t>Some small bent tubing will work</t>
+  </si>
+  <si>
+    <t>HSCDLNN010MDAA3</t>
+  </si>
+  <si>
+    <t>Some tubing for connections</t>
+  </si>
+  <si>
+    <t>Suitable range for measuring BL out to free-stream</t>
+  </si>
+  <si>
+    <t>Instrumented airfoil</t>
+  </si>
+  <si>
+    <t>This unit was custom built with 32 pressure taps on top and bottom, it mounts directly to the lift-drag balance of our wind tunnel. Profile is NACA 0018</t>
+  </si>
+  <si>
+    <t>Instrumented cylinder</t>
+  </si>
+  <si>
+    <t>Works the same as airfoil, but for a smaller tunnel so two experiments can be run at once. Also mounted to a sting for comparison with drag measured via 16 pressure taps</t>
+  </si>
+  <si>
+    <t>Labview data acquisition</t>
+  </si>
+  <si>
+    <t>For measuring lift and drag output from force balance/sting (not pressure taps, those are handled by onboard Particle Photon)</t>
+  </si>
+  <si>
+    <t>Right angle drill head mounted to RC airplane motor (brushless DC?)</t>
+  </si>
+  <si>
+    <t>Custom made part to hold wind turbine models and provide resistive torque to control speed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +196,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,10 +226,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -135,8 +241,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,7 +549,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +601,7 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -492,12 +623,12 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -506,22 +637,22 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -568,4 +699,424 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="6"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="6"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="6"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="6"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="6"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="6"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="6"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="6"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="6"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="6"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="6"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="6"/>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="6"/>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="6"/>
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="6"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="6"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="6"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="6"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="6"/>
+      <c r="C18" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>